<commit_message>
Com close nas telas
</commit_message>
<xml_diff>
--- a/Perfomance_Usuario.XLSX
+++ b/Perfomance_Usuario.XLSX
@@ -25,61 +25,61 @@
     <t>Daniela Fernandes</t>
   </si>
   <si>
+    <t>Adriana Hunhoff</t>
+  </si>
+  <si>
+    <t>Natalia Farias</t>
+  </si>
+  <si>
+    <t>Luana Umpierre</t>
+  </si>
+  <si>
+    <t>Nicolas Silva</t>
+  </si>
+  <si>
     <t>Vania Fagundes</t>
   </si>
   <si>
-    <t>Nicolas Silva</t>
-  </si>
-  <si>
-    <t>Natalia Farias</t>
-  </si>
-  <si>
-    <t>Adriana Hunhoff</t>
-  </si>
-  <si>
-    <t>Luana Umpierre</t>
+    <t>Carlla Bo</t>
+  </si>
+  <si>
+    <t>Julio Acauan</t>
   </si>
   <si>
     <t>Josue Alos</t>
   </si>
   <si>
+    <t>Alexia Pereira</t>
+  </si>
+  <si>
+    <t>Daniel Machado</t>
+  </si>
+  <si>
+    <t>Brenda Pereira</t>
+  </si>
+  <si>
     <t>Amanda Bernardes</t>
   </si>
   <si>
+    <t>Dominique Daudt</t>
+  </si>
+  <si>
+    <t>Eduarda Santos</t>
+  </si>
+  <si>
+    <t>Michele Mattidorff</t>
+  </si>
+  <si>
+    <t>Jonathan Cardoso</t>
+  </si>
+  <si>
+    <t>Gabriel Wolff</t>
+  </si>
+  <si>
+    <t>Gabriel Winter</t>
+  </si>
+  <si>
     <t>Igor Martins</t>
-  </si>
-  <si>
-    <t>Daniel Machado</t>
-  </si>
-  <si>
-    <t>Alexia Pereira</t>
-  </si>
-  <si>
-    <t>Carlla Bo</t>
-  </si>
-  <si>
-    <t>Julio Acauan</t>
-  </si>
-  <si>
-    <t>Brenda Pereira</t>
-  </si>
-  <si>
-    <t>Dominique Daudt</t>
-  </si>
-  <si>
-    <t>Eduarda Santos</t>
-  </si>
-  <si>
-    <t>Michele Mattidorff</t>
-  </si>
-  <si>
-    <t>Jonathan Cardoso</t>
-  </si>
-  <si>
-    <t>Gabriel Wolff</t>
-  </si>
-  <si>
-    <t>Gabriel Winter</t>
   </si>
   <si>
     <t>Brenda Fossa</t>
@@ -542,31 +542,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
       <c r="J2" s="2">
-        <v>150</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -574,31 +574,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>16</v>
+      </c>
+      <c r="G3" s="2">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
       <c r="J3" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -606,31 +606,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>5</v>
       </c>
       <c r="D4" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
       <c r="J4" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -641,28 +641,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E5" s="2">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2">
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J5" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -670,31 +670,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F6" s="2">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="2">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -702,31 +702,31 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F7" s="2">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2">
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="2">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -743,22 +743,22 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" s="2">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="G8" s="2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2">
         <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -775,19 +775,19 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H9" s="2">
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" s="2">
         <v>41</v>
@@ -798,7 +798,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -807,13 +807,13 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
         <v>0</v>
@@ -822,7 +822,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -830,31 +830,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
         <v>2</v>
       </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
       <c r="J11" s="2">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -871,13 +871,13 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -906,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="J13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1278,31 +1278,31 @@
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C25" s="4">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D25" s="4">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="E25" s="4">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F25" s="4">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G25" s="4">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H25" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I25" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J25" s="4">
-        <v>584</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste leitura de tabelas
</commit_message>
<xml_diff>
--- a/Perfomance_Usuario.XLSX
+++ b/Perfomance_Usuario.XLSX
@@ -22,64 +22,64 @@
     <t>Natalia Farias</t>
   </si>
   <si>
+    <t>Daniela Fernandes</t>
+  </si>
+  <si>
+    <t>Vania Fagundes</t>
+  </si>
+  <si>
+    <t>Luana Umpierre</t>
+  </si>
+  <si>
+    <t>Nicolas Silva</t>
+  </si>
+  <si>
+    <t>Adriana Hunhoff</t>
+  </si>
+  <si>
+    <t>Carlla Bo</t>
+  </si>
+  <si>
+    <t>Dominique Daudt</t>
+  </si>
+  <si>
+    <t>Josue Alos</t>
+  </si>
+  <si>
+    <t>Igor Martins</t>
+  </si>
+  <si>
+    <t>Alexia Pereira</t>
+  </si>
+  <si>
+    <t>Gabriel Winter</t>
+  </si>
+  <si>
     <t>Aline Castro</t>
   </si>
   <si>
-    <t>Luana Umpierre</t>
-  </si>
-  <si>
-    <t>Daniela Fernandes</t>
-  </si>
-  <si>
-    <t>Vania Fagundes</t>
-  </si>
-  <si>
-    <t>Nicolas Silva</t>
-  </si>
-  <si>
-    <t>Carlla Bo</t>
-  </si>
-  <si>
-    <t>Dominique Daudt</t>
-  </si>
-  <si>
-    <t>Adriana Hunhoff</t>
+    <t>Julio Acauan</t>
+  </si>
+  <si>
+    <t>Daniel Machado</t>
+  </si>
+  <si>
+    <t>Brenda Pereira</t>
   </si>
   <si>
     <t>Amanda Bernardes</t>
   </si>
   <si>
-    <t>Josue Alos</t>
-  </si>
-  <si>
-    <t>Igor Martins</t>
-  </si>
-  <si>
-    <t>Alexia Pereira</t>
+    <t>Eduarda Santos</t>
   </si>
   <si>
     <t>Michele Mattidorff</t>
   </si>
   <si>
-    <t>Julio Acauan</t>
-  </si>
-  <si>
-    <t>Daniel Machado</t>
-  </si>
-  <si>
-    <t>Brenda Pereira</t>
-  </si>
-  <si>
-    <t>Eduarda Santos</t>
-  </si>
-  <si>
     <t>Jonathan Cardoso</t>
   </si>
   <si>
     <t>Gabriel Wolff</t>
-  </si>
-  <si>
-    <t>Gabriel Winter</t>
   </si>
   <si>
     <t>Brenda Fossa</t>
@@ -547,31 +547,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2">
         <v>12</v>
-      </c>
-      <c r="G2" s="2">
-        <v>8</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="2">
-        <v>77</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -579,31 +579,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
+        <v>66</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
         <v>18</v>
       </c>
-      <c r="E3" s="2">
-        <v>21</v>
-      </c>
-      <c r="F3" s="2">
-        <v>27</v>
-      </c>
       <c r="G3" s="2">
         <v>0</v>
       </c>
       <c r="H3" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="2">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -611,19 +611,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="F4" s="2">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="G4" s="2">
         <v>0</v>
@@ -632,10 +632,10 @@
         <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -643,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -652,10 +652,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
@@ -664,10 +664,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -675,31 +675,31 @@
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="2">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -707,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -716,10 +716,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2">
         <v>0</v>
@@ -728,10 +728,10 @@
         <v>0</v>
       </c>
       <c r="I7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="2">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -739,7 +739,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -748,10 +748,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="G8" s="2">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -780,10 +780,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F9" s="2">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G9" s="2">
         <v>0</v>
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="2">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -803,7 +803,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -812,10 +812,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2">
         <v>0</v>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="2">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -844,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="2">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2">
         <v>0</v>
@@ -859,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="2">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -876,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -908,10 +908,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="2">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -963,7 +963,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2">
         <v>0</v>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2">
         <v>0</v>
@@ -987,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="J15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1016,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1283,31 +1283,31 @@
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C25" s="4">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D25" s="4">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="E25" s="4">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F25" s="4">
-        <v>266</v>
+        <v>204</v>
       </c>
       <c r="G25" s="4">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H25" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I25" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J25" s="4">
-        <v>569</v>
+        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>